<commit_message>
Verified source data, removed older versions of source data and earlier pre-processing scripts
</commit_message>
<xml_diff>
--- a/data/raw/ipeds/Big10_CIP2_2024_20251227.xlsx
+++ b/data/raw/ipeds/Big10_CIP2_2024_20251227.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uillinoisedu-my.sharepoint.com/personal/jswen_illinois_edu/Documents/Documents/Apps/interactive-viz-demo/data/raw/ipeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:40009_{49D9B12C-F8D0-4D65-96A7-162D24BA54F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68E4E557-56BA-4567-B682-B8405C152631}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:40009_{49D9B12C-F8D0-4D65-96A7-162D24BA54F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF1803B4-88C6-4AA2-9FCC-1284F1037A36}"/>
   <bookViews>
-    <workbookView xWindow="-17388" yWindow="-6228" windowWidth="17496" windowHeight="30216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17388" yWindow="-6228" windowWidth="17496" windowHeight="30216" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -894,8 +894,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="17" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -992,18 +992,18 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>64769</xdr:colOff>
+      <xdr:colOff>11429</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
+      <xdr:colOff>182880</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>32385</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="institution name">
@@ -1026,7 +1026,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1036,8 +1036,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="64769" y="167640"/>
-              <a:ext cx="4530091" cy="2425065"/>
+              <a:off x="11429" y="53340"/>
+              <a:ext cx="4530091" cy="2659380"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1070,18 +1070,18 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1335405</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>59055</xdr:rowOff>
+      <xdr:colOff>1007745</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>112395</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="C2024_A.First or Second Major">
@@ -1104,7 +1104,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1114,7 +1114,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4998720" y="194310"/>
+              <a:off x="4671060" y="64770"/>
               <a:ext cx="1861185" cy="2425065"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1148,18 +1148,18 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2221230</xdr:colOff>
+      <xdr:colOff>1116330</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1659255</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>24765</xdr:rowOff>
+      <xdr:colOff>554355</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>116205</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="C2024_A.Award Level code">
@@ -1182,7 +1182,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1192,7 +1192,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7745730" y="160020"/>
+              <a:off x="6640830" y="68580"/>
               <a:ext cx="1899285" cy="2425065"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1225,19 +1225,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>11429</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>681989</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>150495</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>306705</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>512445</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="C2024_A.CIP Code -  2020 Classification">
@@ -1260,7 +1260,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1270,7 +1270,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10458449" y="150495"/>
+              <a:off x="8667749" y="66675"/>
               <a:ext cx="5202556" cy="2745105"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1302,10 +1302,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21195,21 +21191,21 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A17:E46" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="19">
         <item h="1" x="4"/>
-        <item x="8"/>
+        <item h="1" x="8"/>
         <item h="1" x="3"/>
         <item h="1" x="12"/>
         <item h="1" x="14"/>
         <item h="1" x="17"/>
         <item h="1" x="11"/>
         <item h="1" x="0"/>
-        <item h="1" x="2"/>
+        <item x="2"/>
         <item h="1" x="5"/>
         <item h="1" x="6"/>
         <item h="1" x="7"/>
@@ -21225,8 +21221,8 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0">
       <items count="3">
-        <item h="1" x="0"/>
-        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -21317,11 +21313,11 @@
     <pivotField axis="axisCol" showAll="0">
       <items count="7">
         <item h="1" x="5"/>
-        <item x="0"/>
+        <item h="1" x="0"/>
         <item h="1" x="4"/>
         <item h="1" x="3"/>
         <item h="1" x="1"/>
-        <item h="1" x="2"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -21334,10 +21330,13 @@
   </rowFields>
   <rowItems count="27">
     <i>
-      <x v="1"/>
+      <x v="8"/>
     </i>
     <i r="1">
       <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
     </i>
     <i r="1">
       <x v="2"/>
@@ -21352,16 +21351,19 @@
       <x v="5"/>
     </i>
     <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
       <x v="9"/>
     </i>
     <i r="1">
       <x v="10"/>
     </i>
     <i r="1">
-      <x v="12"/>
+      <x v="11"/>
     </i>
     <i r="1">
-      <x v="13"/>
+      <x v="12"/>
     </i>
     <i r="1">
       <x v="14"/>
@@ -21373,13 +21375,7 @@
       <x v="17"/>
     </i>
     <i r="1">
-      <x v="18"/>
-    </i>
-    <i r="1">
       <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
     </i>
     <i r="1">
       <x v="22"/>
@@ -21421,7 +21417,7 @@
   </colFields>
   <colItems count="4">
     <i>
-      <x v="1"/>
+      <x v="5"/>
       <x/>
     </i>
     <i r="1" i="1">
@@ -21459,12 +21455,14 @@
     <tabular pivotCacheId="1353784624">
       <items count="18">
         <i x="4"/>
-        <i x="8" s="1"/>
+        <i x="8"/>
         <i x="3"/>
         <i x="12"/>
+        <i x="14"/>
         <i x="17"/>
+        <i x="11"/>
         <i x="0"/>
-        <i x="2"/>
+        <i x="2" s="1"/>
         <i x="5"/>
         <i x="6"/>
         <i x="7"/>
@@ -21474,8 +21472,6 @@
         <i x="1"/>
         <i x="15"/>
         <i x="16"/>
-        <i x="14" nd="1"/>
-        <i x="11" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -21490,8 +21486,8 @@
   <data>
     <tabular pivotCacheId="1353784624">
       <items count="2">
-        <i x="0"/>
-        <i x="1" s="1"/>
+        <i x="0" s="1"/>
+        <i x="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -21506,12 +21502,12 @@
   <data>
     <tabular pivotCacheId="1353784624">
       <items count="6">
-        <i x="0" s="1"/>
+        <i x="0"/>
+        <i x="3"/>
         <i x="1"/>
+        <i x="2" s="1"/>
         <i x="5" nd="1"/>
         <i x="4" nd="1"/>
-        <i x="3" nd="1"/>
-        <i x="2" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -21528,15 +21524,16 @@
       <items count="37">
         <i x="31" s="1"/>
         <i x="0" s="1"/>
+        <i x="1" s="1"/>
         <i x="2" s="1"/>
         <i x="3" s="1"/>
+        <i x="4" s="1"/>
         <i x="5" s="1"/>
         <i x="6" s="1"/>
+        <i x="26" s="1"/>
         <i x="7" s="1"/>
-        <i x="27" s="1"/>
         <i x="8" s="1"/>
         <i x="9" s="1"/>
-        <i x="10" s="1"/>
         <i x="12" s="1"/>
         <i x="13" s="1"/>
         <i x="14" s="1"/>
@@ -21544,7 +21541,6 @@
         <i x="15" s="1"/>
         <i x="16" s="1"/>
         <i x="17" s="1"/>
-        <i x="30" s="1"/>
         <i x="18" s="1"/>
         <i x="19" s="1"/>
         <i x="20" s="1"/>
@@ -21552,15 +21548,15 @@
         <i x="22" s="1"/>
         <i x="23" s="1"/>
         <i x="24"/>
-        <i x="1" s="1" nd="1"/>
         <i x="25" s="1" nd="1"/>
-        <i x="4" s="1" nd="1"/>
         <i x="35" s="1" nd="1"/>
-        <i x="26" s="1" nd="1"/>
+        <i x="27" s="1" nd="1"/>
+        <i x="10" s="1" nd="1"/>
         <i x="11" s="1" nd="1"/>
         <i x="33" s="1" nd="1"/>
         <i x="29" s="1" nd="1"/>
         <i x="32" s="1" nd="1"/>
+        <i x="30" s="1" nd="1"/>
         <i x="34" s="1" nd="1"/>
         <i x="36" s="1" nd="1"/>
       </items>
@@ -21895,8 +21891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A17:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21917,7 +21913,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>113</v>
@@ -21939,18 +21935,18 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="9">
-        <v>336</v>
-      </c>
-      <c r="C20" s="10">
+        <v>80</v>
+      </c>
+      <c r="B20" s="10">
+        <v>6489</v>
+      </c>
+      <c r="C20" s="9">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
-        <v>336</v>
-      </c>
-      <c r="E20" s="10">
+      <c r="D20" s="10">
+        <v>6489</v>
+      </c>
+      <c r="E20" s="9">
         <v>1</v>
       </c>
     </row>
@@ -21958,441 +21954,441 @@
       <c r="A21" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="9">
-        <v>2</v>
-      </c>
-      <c r="C21" s="10">
-        <v>5.9523809523809521E-3</v>
-      </c>
-      <c r="D21" s="9">
-        <v>2</v>
-      </c>
-      <c r="E21" s="10">
-        <v>5.9523809523809521E-3</v>
+      <c r="B21" s="10">
+        <v>135</v>
+      </c>
+      <c r="C21" s="9">
+        <v>2.0804438280166437E-2</v>
+      </c>
+      <c r="D21" s="10">
+        <v>135</v>
+      </c>
+      <c r="E21" s="9">
+        <v>2.0804438280166437E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="9">
-        <v>2</v>
-      </c>
-      <c r="C22" s="10">
-        <v>5.9523809523809521E-3</v>
-      </c>
-      <c r="D22" s="9">
-        <v>2</v>
-      </c>
-      <c r="E22" s="10">
-        <v>5.9523809523809521E-3</v>
+        <v>16</v>
+      </c>
+      <c r="B22" s="10">
+        <v>81</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1.2482662968099861E-2</v>
+      </c>
+      <c r="D22" s="10">
+        <v>81</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1.2482662968099861E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="9">
-        <v>34</v>
-      </c>
-      <c r="C23" s="10">
-        <v>0.10119047619047619</v>
-      </c>
-      <c r="D23" s="9">
-        <v>34</v>
-      </c>
-      <c r="E23" s="10">
-        <v>0.10119047619047619</v>
+        <v>19</v>
+      </c>
+      <c r="B23" s="10">
+        <v>12</v>
+      </c>
+      <c r="C23" s="9">
+        <v>1.8492834026814608E-3</v>
+      </c>
+      <c r="D23" s="10">
+        <v>12</v>
+      </c>
+      <c r="E23" s="9">
+        <v>1.8492834026814608E-3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="9">
-        <v>2</v>
-      </c>
-      <c r="C24" s="10">
-        <v>5.9523809523809521E-3</v>
-      </c>
-      <c r="D24" s="9">
-        <v>2</v>
-      </c>
-      <c r="E24" s="10">
-        <v>5.9523809523809521E-3</v>
+        <v>40</v>
+      </c>
+      <c r="B24" s="10">
+        <v>70</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1.0787486515641856E-2</v>
+      </c>
+      <c r="D24" s="10">
+        <v>70</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1.0787486515641856E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="9">
-        <v>22</v>
-      </c>
-      <c r="C25" s="10">
-        <v>6.5476190476190479E-2</v>
-      </c>
-      <c r="D25" s="9">
-        <v>22</v>
-      </c>
-      <c r="E25" s="10">
-        <v>6.5476190476190479E-2</v>
+        <v>60</v>
+      </c>
+      <c r="B25" s="10">
+        <v>2569</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.39590075512405609</v>
+      </c>
+      <c r="D25" s="10">
+        <v>2569</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0.39590075512405609</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="9">
-        <v>6</v>
-      </c>
-      <c r="C26" s="10">
-        <v>1.7857142857142856E-2</v>
-      </c>
-      <c r="D26" s="9">
-        <v>6</v>
-      </c>
-      <c r="E26" s="10">
-        <v>1.7857142857142856E-2</v>
+        <v>21</v>
+      </c>
+      <c r="B26" s="10">
+        <v>39</v>
+      </c>
+      <c r="C26" s="9">
+        <v>6.0101710587147483E-3</v>
+      </c>
+      <c r="D26" s="10">
+        <v>39</v>
+      </c>
+      <c r="E26" s="9">
+        <v>6.0101710587147483E-3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="9">
-        <v>5</v>
-      </c>
-      <c r="C27" s="10">
-        <v>1.488095238095238E-2</v>
-      </c>
-      <c r="D27" s="9">
-        <v>5</v>
-      </c>
-      <c r="E27" s="10">
-        <v>1.488095238095238E-2</v>
+        <v>23</v>
+      </c>
+      <c r="B27" s="10">
+        <v>1462</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.22530436122669131</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1462</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0.22530436122669131</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="9">
-        <v>4</v>
-      </c>
-      <c r="C28" s="10">
-        <v>1.1904761904761904E-2</v>
-      </c>
-      <c r="D28" s="9">
-        <v>4</v>
-      </c>
-      <c r="E28" s="10">
-        <v>1.1904761904761904E-2</v>
+        <v>25</v>
+      </c>
+      <c r="B28" s="10">
+        <v>224</v>
+      </c>
+      <c r="C28" s="9">
+        <v>3.4519956850053934E-2</v>
+      </c>
+      <c r="D28" s="10">
+        <v>224</v>
+      </c>
+      <c r="E28" s="9">
+        <v>3.4519956850053934E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="9">
-        <v>1</v>
-      </c>
-      <c r="C29" s="10">
-        <v>2.976190476190476E-3</v>
-      </c>
-      <c r="D29" s="9">
-        <v>1</v>
-      </c>
-      <c r="E29" s="10">
-        <v>2.976190476190476E-3</v>
+        <v>27</v>
+      </c>
+      <c r="B29" s="10">
+        <v>654</v>
+      </c>
+      <c r="C29" s="9">
+        <v>0.10078594544613963</v>
+      </c>
+      <c r="D29" s="10">
+        <v>654</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0.10078594544613963</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="9">
-        <v>39</v>
-      </c>
-      <c r="C30" s="10">
-        <v>0.11607142857142858</v>
-      </c>
-      <c r="D30" s="9">
-        <v>39</v>
-      </c>
-      <c r="E30" s="10">
-        <v>0.11607142857142858</v>
+        <v>71</v>
+      </c>
+      <c r="B30" s="10">
+        <v>63</v>
+      </c>
+      <c r="C30" s="9">
+        <v>9.7087378640776691E-3</v>
+      </c>
+      <c r="D30" s="10">
+        <v>63</v>
+      </c>
+      <c r="E30" s="9">
+        <v>9.7087378640776691E-3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="9">
-        <v>4</v>
-      </c>
-      <c r="C31" s="10">
-        <v>1.1904761904761904E-2</v>
-      </c>
-      <c r="D31" s="9">
-        <v>4</v>
-      </c>
-      <c r="E31" s="10">
-        <v>1.1904761904761904E-2</v>
+        <v>34</v>
+      </c>
+      <c r="B31" s="10">
+        <v>10</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1.5410695022345508E-3</v>
+      </c>
+      <c r="D31" s="10">
+        <v>10</v>
+      </c>
+      <c r="E31" s="9">
+        <v>1.5410695022345508E-3</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="9">
-        <v>7</v>
-      </c>
-      <c r="C32" s="10">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D32" s="9">
-        <v>7</v>
-      </c>
-      <c r="E32" s="10">
-        <v>2.0833333333333332E-2</v>
+        <v>29</v>
+      </c>
+      <c r="B32" s="10">
+        <v>40</v>
+      </c>
+      <c r="C32" s="9">
+        <v>6.1642780089382031E-3</v>
+      </c>
+      <c r="D32" s="10">
+        <v>40</v>
+      </c>
+      <c r="E32" s="9">
+        <v>6.1642780089382031E-3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="9">
-        <v>28</v>
-      </c>
-      <c r="C33" s="10">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="D33" s="9">
-        <v>28</v>
-      </c>
-      <c r="E33" s="10">
-        <v>8.3333333333333329E-2</v>
+        <v>58</v>
+      </c>
+      <c r="B33" s="10">
+        <v>75</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1.155802126675913E-2</v>
+      </c>
+      <c r="D33" s="10">
+        <v>75</v>
+      </c>
+      <c r="E33" s="9">
+        <v>1.155802126675913E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="9">
-        <v>5</v>
-      </c>
-      <c r="C34" s="10">
-        <v>1.488095238095238E-2</v>
-      </c>
-      <c r="D34" s="9">
-        <v>5</v>
-      </c>
-      <c r="E34" s="10">
-        <v>1.488095238095238E-2</v>
+        <v>62</v>
+      </c>
+      <c r="B34" s="10">
+        <v>6</v>
+      </c>
+      <c r="C34" s="9">
+        <v>9.2464170134073042E-4</v>
+      </c>
+      <c r="D34" s="10">
+        <v>6</v>
+      </c>
+      <c r="E34" s="9">
+        <v>9.2464170134073042E-4</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="9">
-        <v>1</v>
-      </c>
-      <c r="C35" s="10">
-        <v>2.976190476190476E-3</v>
-      </c>
-      <c r="D35" s="9">
-        <v>1</v>
-      </c>
-      <c r="E35" s="10">
-        <v>2.976190476190476E-3</v>
+        <v>31</v>
+      </c>
+      <c r="B35" s="10">
+        <v>88</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1.3561411619664046E-2</v>
+      </c>
+      <c r="D35" s="10">
+        <v>88</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1.3561411619664046E-2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="9">
-        <v>11</v>
-      </c>
-      <c r="C36" s="10">
-        <v>3.273809523809524E-2</v>
-      </c>
-      <c r="D36" s="9">
-        <v>11</v>
-      </c>
-      <c r="E36" s="10">
-        <v>3.273809523809524E-2</v>
+      <c r="B36" s="10">
+        <v>289</v>
+      </c>
+      <c r="C36" s="9">
+        <v>4.453690861457852E-2</v>
+      </c>
+      <c r="D36" s="10">
+        <v>289</v>
+      </c>
+      <c r="E36" s="9">
+        <v>4.453690861457852E-2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="9">
-        <v>16</v>
-      </c>
-      <c r="C37" s="10">
-        <v>4.7619047619047616E-2</v>
-      </c>
-      <c r="D37" s="9">
-        <v>16</v>
-      </c>
-      <c r="E37" s="10">
-        <v>4.7619047619047616E-2</v>
+      <c r="B37" s="10">
+        <v>189</v>
+      </c>
+      <c r="C37" s="9">
+        <v>2.9126213592233011E-2</v>
+      </c>
+      <c r="D37" s="10">
+        <v>189</v>
+      </c>
+      <c r="E37" s="9">
+        <v>2.9126213592233011E-2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="9">
-        <v>2</v>
-      </c>
-      <c r="C38" s="10">
-        <v>5.9523809523809521E-3</v>
-      </c>
-      <c r="D38" s="9">
-        <v>2</v>
-      </c>
-      <c r="E38" s="10">
-        <v>5.9523809523809521E-3</v>
+      <c r="B38" s="10">
+        <v>33</v>
+      </c>
+      <c r="C38" s="9">
+        <v>5.0855293573740176E-3</v>
+      </c>
+      <c r="D38" s="10">
+        <v>33</v>
+      </c>
+      <c r="E38" s="9">
+        <v>5.0855293573740176E-3</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="9">
-        <v>2</v>
-      </c>
-      <c r="C39" s="10">
-        <v>5.9523809523809521E-3</v>
-      </c>
-      <c r="D39" s="9">
-        <v>2</v>
-      </c>
-      <c r="E39" s="10">
-        <v>5.9523809523809521E-3</v>
+      <c r="B39" s="10">
+        <v>34</v>
+      </c>
+      <c r="C39" s="9">
+        <v>5.2396363075974724E-3</v>
+      </c>
+      <c r="D39" s="10">
+        <v>34</v>
+      </c>
+      <c r="E39" s="9">
+        <v>5.2396363075974724E-3</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="9">
-        <v>1</v>
-      </c>
-      <c r="C40" s="10">
-        <v>2.976190476190476E-3</v>
-      </c>
-      <c r="D40" s="9">
-        <v>1</v>
-      </c>
-      <c r="E40" s="10">
-        <v>2.976190476190476E-3</v>
+      <c r="B40" s="10">
+        <v>3</v>
+      </c>
+      <c r="C40" s="9">
+        <v>4.6232085067036521E-4</v>
+      </c>
+      <c r="D40" s="10">
+        <v>3</v>
+      </c>
+      <c r="E40" s="9">
+        <v>4.6232085067036521E-4</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="9">
-        <v>5</v>
-      </c>
-      <c r="C41" s="10">
-        <v>1.488095238095238E-2</v>
-      </c>
-      <c r="D41" s="9">
-        <v>5</v>
-      </c>
-      <c r="E41" s="10">
-        <v>1.488095238095238E-2</v>
+      <c r="B41" s="10">
+        <v>43</v>
+      </c>
+      <c r="C41" s="9">
+        <v>6.6265988596085684E-3</v>
+      </c>
+      <c r="D41" s="10">
+        <v>43</v>
+      </c>
+      <c r="E41" s="9">
+        <v>6.6265988596085684E-3</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="9">
-        <v>79</v>
-      </c>
-      <c r="C42" s="10">
-        <v>0.23511904761904762</v>
-      </c>
-      <c r="D42" s="9">
-        <v>79</v>
-      </c>
-      <c r="E42" s="10">
-        <v>0.23511904761904762</v>
+      <c r="B42" s="10">
+        <v>20</v>
+      </c>
+      <c r="C42" s="9">
+        <v>3.0821390044691015E-3</v>
+      </c>
+      <c r="D42" s="10">
+        <v>20</v>
+      </c>
+      <c r="E42" s="9">
+        <v>3.0821390044691015E-3</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="9">
-        <v>1</v>
-      </c>
-      <c r="C43" s="10">
-        <v>2.976190476190476E-3</v>
-      </c>
-      <c r="D43" s="9">
-        <v>1</v>
-      </c>
-      <c r="E43" s="10">
-        <v>2.976190476190476E-3</v>
+      <c r="B43" s="10">
+        <v>183</v>
+      </c>
+      <c r="C43" s="9">
+        <v>2.8201571890892278E-2</v>
+      </c>
+      <c r="D43" s="10">
+        <v>183</v>
+      </c>
+      <c r="E43" s="9">
+        <v>2.8201571890892278E-2</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="9">
-        <v>45</v>
-      </c>
-      <c r="C44" s="10">
-        <v>0.13392857142857142</v>
-      </c>
-      <c r="D44" s="9">
-        <v>45</v>
-      </c>
-      <c r="E44" s="10">
-        <v>0.13392857142857142</v>
+      <c r="B44" s="10">
+        <v>103</v>
+      </c>
+      <c r="C44" s="9">
+        <v>1.5873015873015872E-2</v>
+      </c>
+      <c r="D44" s="10">
+        <v>103</v>
+      </c>
+      <c r="E44" s="9">
+        <v>1.5873015873015872E-2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="9">
-        <v>12</v>
-      </c>
-      <c r="C45" s="10">
-        <v>3.5714285714285712E-2</v>
-      </c>
-      <c r="D45" s="9">
-        <v>12</v>
-      </c>
-      <c r="E45" s="10">
-        <v>3.5714285714285712E-2</v>
+      <c r="B45" s="10">
+        <v>64</v>
+      </c>
+      <c r="C45" s="9">
+        <v>9.8628448143011256E-3</v>
+      </c>
+      <c r="D45" s="10">
+        <v>64</v>
+      </c>
+      <c r="E45" s="9">
+        <v>9.8628448143011256E-3</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="9">
-        <v>336</v>
-      </c>
-      <c r="C46" s="10">
+      <c r="B46" s="10">
+        <v>6489</v>
+      </c>
+      <c r="C46" s="9">
         <v>1</v>
       </c>
-      <c r="D46" s="9">
-        <v>336</v>
-      </c>
-      <c r="E46" s="10">
+      <c r="D46" s="10">
+        <v>6489</v>
+      </c>
+      <c r="E46" s="9">
         <v>1</v>
       </c>
     </row>
@@ -22413,7 +22409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I1795"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>